<commit_message>
ready for extract most of the data
Signed-off-by: Masrik Dahir <dahirma@vcu.edu>
</commit_message>
<xml_diff>
--- a/my-xlsx-file.xlsx
+++ b/my-xlsx-file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>User Id</t>
   </si>
@@ -40,6 +40,18 @@
     <t>Longitude</t>
   </si>
   <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>County/Suburb/Neighbourhood/City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
     <t>Midday LFP FBFK</t>
   </si>
   <si>
@@ -49,10 +61,22 @@
     <t>Shipping Address 4602 76th Ave Ct NWGig Harbor, WA 98335</t>
   </si>
   <si>
-    <t>473404659</t>
-  </si>
-  <si>
-    <t>1227429631</t>
+    <t>47.3404659</t>
+  </si>
+  <si>
+    <t>-122.7429631</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92nd Street NW</t>
+  </si>
+  <si>
+    <t>Pierce County</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>98394</t>
   </si>
   <si>
     <t>AMSS Clinic Pantry</t>
@@ -61,10 +85,22 @@
     <t>Shipping Address 588 Wilma StreetLongwood FL 32750</t>
   </si>
   <si>
-    <t>286973858</t>
-  </si>
-  <si>
-    <t>8134892219999999</t>
+    <t>28.6973858</t>
+  </si>
+  <si>
+    <t>-81.34892219999999</t>
+  </si>
+  <si>
+    <t>213 Short Avenue</t>
+  </si>
+  <si>
+    <t>Seminole County</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>32750</t>
   </si>
   <si>
     <t>Little Free Pantry</t>
@@ -76,10 +112,22 @@
     <t>Contact Peace Lutheran Church (office@peaceelca.org)</t>
   </si>
   <si>
-    <t>428125002</t>
-  </si>
-  <si>
-    <t>861253223</t>
+    <t>42.8125002</t>
+  </si>
+  <si>
+    <t>-86.1253223</t>
+  </si>
+  <si>
+    <t>397 James Street</t>
+  </si>
+  <si>
+    <t>Ottawa County</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>49424</t>
   </si>
   <si>
     <t>First Baptist Church of Edwardsville</t>
@@ -91,10 +139,22 @@
     <t>Contact office@edfbc.org</t>
   </si>
   <si>
-    <t>388106515</t>
-  </si>
-  <si>
-    <t>8996231519999999</t>
+    <t>38.8106515</t>
+  </si>
+  <si>
+    <t>-89.96231519999999</t>
+  </si>
+  <si>
+    <t>534 Saint Louis Street</t>
+  </si>
+  <si>
+    <t>Madison County</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>62025</t>
   </si>
   <si>
     <t>Broadmoor Community Church Pantry</t>
@@ -106,10 +166,22 @@
     <t>Contact Patrick Johnson (patrickk84@gmail.com)</t>
   </si>
   <si>
-    <t>387943971</t>
-  </si>
-  <si>
-    <t>1048325652</t>
+    <t>38.7943971</t>
+  </si>
+  <si>
+    <t>-104.8325652</t>
+  </si>
+  <si>
+    <t>175 Lake Avenue</t>
+  </si>
+  <si>
+    <t>El Paso County</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>80906</t>
   </si>
   <si>
     <t>Oconee Presbyterian Church Little Free Pantry</t>
@@ -118,19 +190,43 @@
     <t>Shipping Address Missions Elderc/o Oconee Presbyterian Church2601 Hog Mountain RdWatkinsville, GA 30677</t>
   </si>
   <si>
-    <t>338637111</t>
-  </si>
-  <si>
-    <t>8345122479999999</t>
+    <t>33.8637111</t>
+  </si>
+  <si>
+    <t>-83.45122479999999</t>
+  </si>
+  <si>
+    <t>2601 Hog Mountain Road</t>
+  </si>
+  <si>
+    <t>Oconee County</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>30677</t>
   </si>
   <si>
     <t>Shipping Address 203 St Pauls AveStaten Island, NY 10304</t>
   </si>
   <si>
-    <t>406326597</t>
-  </si>
-  <si>
-    <t>740788226</t>
+    <t>40.6326597</t>
+  </si>
+  <si>
+    <t>-74.0788226</t>
+  </si>
+  <si>
+    <t>203 Saint Pauls Avenue</t>
+  </si>
+  <si>
+    <t>Staten Island</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>10304</t>
   </si>
   <si>
     <t>West Bay Blessing Box</t>
@@ -139,25 +235,52 @@
     <t>Shipping Address West Bay Advent Christian Church6326 Laird Park Rd. Panama City Beach, FL 32413</t>
   </si>
   <si>
-    <t>302911565</t>
-  </si>
-  <si>
-    <t>858596391</t>
+    <t>30.2911565</t>
+  </si>
+  <si>
+    <t>-85.8596391</t>
+  </si>
+  <si>
+    <t>6326 Laird Park Road</t>
+  </si>
+  <si>
+    <t>Bay County</t>
+  </si>
+  <si>
+    <t>32413</t>
   </si>
   <si>
     <t>McKinney Little Free Pantry</t>
   </si>
   <si>
-    <t>332006375</t>
-  </si>
-  <si>
-    <t>966023039</t>
-  </si>
-  <si>
-    <t>331939048</t>
-  </si>
-  <si>
-    <t>966475057</t>
+    <t>33.2006375</t>
+  </si>
+  <si>
+    <t>-96.6023039</t>
+  </si>
+  <si>
+    <t>436 Lincoln Street</t>
+  </si>
+  <si>
+    <t>Collin County</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>75069</t>
+  </si>
+  <si>
+    <t>33.1939048</t>
+  </si>
+  <si>
+    <t>-96.6475057</t>
+  </si>
+  <si>
+    <t>642 Blue Ridge Street</t>
+  </si>
+  <si>
+    <t>75072</t>
   </si>
 </sst>
 </file>
@@ -489,13 +612,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,214 +643,346 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>80</v>
+      </c>
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>86</v>
+      </c>
+      <c r="I11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>